<commit_message>
late save on excel file
</commit_message>
<xml_diff>
--- a/assets/data/formatdata.xlsx
+++ b/assets/data/formatdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bscript/projects/devry/ceis110/weather-api/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7260A76C-2802-4C4A-86EF-9EE286E1D6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5D55D167-D91F-ED4F-ACF4-9B10C7274BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29440" yWindow="7620" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="10200" yWindow="4380" windowWidth="30400" windowHeight="19560"/>
   </bookViews>
   <sheets>
     <sheet name="formatdata" sheetId="1" r:id="rId1"/>
@@ -572,6 +572,2000 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Temperature</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> and Humidity</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>formatdata!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Celsius</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>formatdata!$A$2:$A$111</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="110"/>
+                <c:pt idx="0">
+                  <c:v>14.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>14.4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>16.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>16.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>15.6</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13.9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12.2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>14.4</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>14.4</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>13.9</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>12.2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>9.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A56-8747-9B26-1697E0C07A0A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>formatdata!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Fahrenheit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>formatdata!$B$2:$B$111</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="110"/>
+                <c:pt idx="0">
+                  <c:v>57.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55.04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.06</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48.92</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>48.92</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48.02</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48.02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46.94</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>46.94</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>46.94</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>46.04</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44.96</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>46.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>46.4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>48.02</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>51.98</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>55.04</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>57.92</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>60.08</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>60.98</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>60.98</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>60.08</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>57.02</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>55.04</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>53.96</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>53.06</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>51.08</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>48.92</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>48.02</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>48.02</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>48.02</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>48.02</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>48.2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>48.92</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>48.92</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>48.92</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>48.2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>51.08</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51.8</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>51.8</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>51.08</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>51.8</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>51.98</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>51.8</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>51.8</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>51.98</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>51.8</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>51.08</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>51.8</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>51.8</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>51.8</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>51.98</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>53.6</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>51.98</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>51.8</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>53.06</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>53.6</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>53.06</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>53.06</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>51.08</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>48.92</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>48.2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>48.02</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>46.94</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>46.94</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>44.96</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>44.96</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>46.04</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>46.04</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>44.6</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>42.8</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>44.06</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>44.96</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>44.96</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>46.4</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>46.04</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>46.4</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>46.4</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>46.94</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>48.02</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>48.2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>51.08</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>53.06</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>55.94</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>55.4</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>57.92</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>57.92</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>57.02</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>55.94</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>53.96</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>53.06</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>51.98</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>51.8</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>51.08</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>48.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7A56-8747-9B26-1697E0C07A0A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>formatdata!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Humidity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>formatdata!$C$2:$C$111</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="110"/>
+                <c:pt idx="0">
+                  <c:v>71.923565721952997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79.811182429167005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.654510078887995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85.680481185637007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89.181204957654003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89.741574390528001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>86.141284587184998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>89.091584214285007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>89.091584214285007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>92.815182297915996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>96.659876800571993</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92.782035663943006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>92.782035663943006</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>95.988158411756999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>92.815182297915996</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>86.313549377715006</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>79.811182429167005</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>74.876463020299994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>66.579992947826</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>75.162754589756005</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>72.237265552403002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>74.582928368531</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>80.500571981250999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>79.811182429167005</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>83.015085466252003</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>82.954048467221</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>85.680481185637007</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>89.181204957654003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>89.181204957654003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>89.741574390528001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>92.815182297915996</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>96.022450441781004</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>96.022450441781004</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>96.022450441781004</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>93.453994643447999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>92.842632704447993</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>92.842632704447993</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>92.842632704447993</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>93.504015298216004</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>89.181204957654003</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>93.504015298216004</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>92.875368778185006</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>92.285708289197004</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>87.476252351683002</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>93.504015298216004</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>87.476252351683002</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>92.285708289197004</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>87.476252351683002</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>89.269748995157997</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>87.476252351683002</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>93.553471551667002</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>89.269748995157997</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>87.476252351683002</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>92.285708289197004</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>87.476252351683002</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>87.476252351683002</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>87.476252351683002</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>86.313549377715006</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>81.879846925107003</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>82.880385175757993</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>81.750052187031002</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>79.654510078887995</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>76.519987759453002</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>79.654510078887995</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>76.993951308353004</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>79.496094610696005</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>79.870781661167996</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>81.486420017859004</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>86.090017231195006</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>86.028130972357005</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>86.028130972357005</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>92.720676321385994</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>92.720676321385994</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>92.754240308299998</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>92.754240308299998</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>93.352225938757002</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>95.953424201416993</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>96.630919733260001</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>96.630919733260001</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>93.403401079212998</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>92.754240308299998</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>93.403401079212998</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>93.403401079212998</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92.782035663943006</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>92.815182297915996</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>93.453994643447999</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>82.818647556174994</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>76.993951308353004</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>66.541382376325998</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>71.661522629146006</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>64.545340236686002</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>59.604608806526997</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>59.604608806526997</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>59.868539990945997</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>61.838774319797999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>66.541382376325998</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>71.510261021778007</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>73.905075949332996</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>74.307349532130999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>76.357329126718</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>73.709316572125999</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>77.156442416889007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7A56-8747-9B26-1697E0C07A0A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1577934720"/>
+        <c:axId val="1263603232"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1577934720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1263603232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1263603232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1577934720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E1FC0F4-36CE-404A-A066-C031773594AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -869,9 +2863,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="G100" sqref="G100"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1920,59 +3916,70 @@
         <v>93.453994643447999</v>
       </c>
     </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>10.6</v>
+      </c>
+      <c r="B96">
+        <v>51.08</v>
+      </c>
+      <c r="C96">
+        <v>82.818647556174994</v>
+      </c>
+    </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>10.6</v>
+        <v>11.7</v>
       </c>
       <c r="B97">
-        <v>51.08</v>
+        <v>53.06</v>
       </c>
       <c r="C97">
-        <v>82.818647556174994</v>
+        <v>76.993951308353004</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>11.7</v>
+        <v>13.3</v>
       </c>
       <c r="B98">
-        <v>53.06</v>
+        <v>55.94</v>
       </c>
       <c r="C98">
-        <v>76.993951308353004</v>
+        <v>66.541382376325998</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>13.3</v>
+        <v>13</v>
       </c>
       <c r="B99">
-        <v>55.94</v>
+        <v>55.4</v>
       </c>
       <c r="C99">
-        <v>66.541382376325998</v>
+        <v>71.661522629146006</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>13</v>
+        <v>14.4</v>
       </c>
       <c r="B100">
-        <v>55.4</v>
+        <v>57.92</v>
       </c>
       <c r="C100">
-        <v>71.661522629146006</v>
+        <v>64.545340236686002</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>14.4</v>
+        <v>15</v>
       </c>
       <c r="B101">
-        <v>57.92</v>
+        <v>59</v>
       </c>
       <c r="C101">
-        <v>64.545340236686002</v>
+        <v>59.604608806526997</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -1988,115 +3995,105 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>15</v>
+        <v>14.4</v>
       </c>
       <c r="B103">
-        <v>59</v>
+        <v>57.92</v>
       </c>
       <c r="C103">
-        <v>59.604608806526997</v>
+        <v>59.868539990945997</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>14.4</v>
+        <v>13.9</v>
       </c>
       <c r="B104">
-        <v>57.92</v>
+        <v>57.02</v>
       </c>
       <c r="C104">
-        <v>59.868539990945997</v>
+        <v>61.838774319797999</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>13.9</v>
+        <v>13.3</v>
       </c>
       <c r="B105">
-        <v>57.02</v>
+        <v>55.94</v>
       </c>
       <c r="C105">
-        <v>61.838774319797999</v>
+        <v>66.541382376325998</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>13.3</v>
+        <v>12.2</v>
       </c>
       <c r="B106">
-        <v>55.94</v>
+        <v>53.96</v>
       </c>
       <c r="C106">
-        <v>66.541382376325998</v>
+        <v>71.510261021778007</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>12.2</v>
+        <v>11.7</v>
       </c>
       <c r="B107">
-        <v>53.96</v>
+        <v>53.06</v>
       </c>
       <c r="C107">
-        <v>71.510261021778007</v>
+        <v>73.905075949332996</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>11.7</v>
+        <v>11.1</v>
       </c>
       <c r="B108">
-        <v>53.06</v>
+        <v>51.98</v>
       </c>
       <c r="C108">
-        <v>73.905075949332996</v>
+        <v>74.307349532130999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>11</v>
+      </c>
+      <c r="B109">
+        <v>51.8</v>
+      </c>
+      <c r="C109">
+        <v>76.357329126718</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>11.1</v>
+        <v>10.6</v>
       </c>
       <c r="B110">
-        <v>51.98</v>
+        <v>51.08</v>
       </c>
       <c r="C110">
-        <v>74.307349532130999</v>
+        <v>73.709316572125999</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>11</v>
+        <v>9.4</v>
       </c>
       <c r="B111">
-        <v>51.8</v>
+        <v>48.92</v>
       </c>
       <c r="C111">
-        <v>76.357329126718</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112">
-        <v>10.6</v>
-      </c>
-      <c r="B112">
-        <v>51.08</v>
-      </c>
-      <c r="C112">
-        <v>73.709316572125999</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113">
-        <v>9.4</v>
-      </c>
-      <c r="B113">
-        <v>48.92</v>
-      </c>
-      <c r="C113">
         <v>77.156442416889007</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>